<commit_message>
add search engine for text file and edit blob for more than 1 rivers
</commit_message>
<xml_diff>
--- a/Semaster 2/OOP/Recursion/blob.xlsx
+++ b/Semaster 2/OOP/Recursion/blob.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UBIT-Work\Semaster 2\OOP\Recursion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huzai\OneDrive\Documents\GitHub\UBIT-Work\Semaster 2\OOP\Recursion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F65F5531-3E7F-40D9-9B11-F8D14E9D89DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C489ED82-A30E-4356-B2B7-D14F8A74DCD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1F94C753-C621-4359-8994-6558598E46ED}"/>
   </bookViews>
@@ -61,7 +61,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -69,66 +69,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -442,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69C0A3F-A964-41CA-B2B7-732014D27FDF}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,13 +645,13 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -749,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -796,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -843,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -890,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -937,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -984,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1031,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1078,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1125,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1172,10 +1112,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1222,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1269,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1313,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1360,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1407,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1454,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1501,10 +1441,10 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1551,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1592,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1601,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1642,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1651,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1692,13 +1632,13 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1739,13 +1679,13 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1786,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1858,6 +1798,12 @@
       </c>
       <c r="O30">
         <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f>COUNTIF(A1:O30,"=1")</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add quick sort and update blob code to count more than one rivers
</commit_message>
<xml_diff>
--- a/Semaster 2/OOP/Recursion/blob.xlsx
+++ b/Semaster 2/OOP/Recursion/blob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huzai\OneDrive\Documents\GitHub\UBIT-Work\Semaster 2\OOP\Recursion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C489ED82-A30E-4356-B2B7-D14F8A74DCD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9337E757-FE1B-4E2A-A52D-8F07C0CCF44C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1F94C753-C621-4359-8994-6558598E46ED}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection sqref="A1:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1538,10 +1538,10 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1682,10 +1682,10 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1803,7 +1803,7 @@
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34">
         <f>COUNTIF(A1:O30,"=1")</f>
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>